<commit_message>
Revert "Revert "Update template""
This reverts commit 5696ee911903195b57e47183129e6060de80224d.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,11 +8,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miWhAMakEOtnWiDKgAnpnoc3yXvGw=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="163">
   <si>
     <t>i</t>
   </si>
@@ -254,245 +259,260 @@
     <t>c24</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>g25</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>ɲ</t>
+  </si>
+  <si>
+    <t>c25</t>
+  </si>
+  <si>
     <t>beat</t>
   </si>
   <si>
-    <t>/b/i/t/</t>
-  </si>
-  <si>
     <t>bit</t>
   </si>
   <si>
-    <t>/b/ɪ/t/</t>
+    <t>bɪt</t>
   </si>
   <si>
     <t>bait</t>
   </si>
   <si>
-    <t>/b/e/t/</t>
-  </si>
-  <si>
     <t>bet</t>
   </si>
   <si>
-    <t>/b/ɛ/t/</t>
+    <t>bɛt</t>
   </si>
   <si>
     <t>bat</t>
   </si>
   <si>
-    <t>/b/æ/t/</t>
+    <t>bæt</t>
   </si>
   <si>
     <t>but</t>
   </si>
   <si>
-    <t>/b/ʌ/t/</t>
+    <t>bʌt</t>
   </si>
   <si>
     <t>about</t>
   </si>
   <si>
-    <t>/ə/b/o/t/</t>
+    <t>əbot</t>
   </si>
   <si>
     <t>bird</t>
   </si>
   <si>
-    <t>/b/ɚ/d/</t>
+    <t>bɚd</t>
   </si>
   <si>
     <t>boot</t>
   </si>
   <si>
-    <t>/b/u/t/</t>
-  </si>
-  <si>
     <t>book</t>
   </si>
   <si>
-    <t>/b/ʊ/k/</t>
+    <t>bʊk</t>
   </si>
   <si>
     <t>boat</t>
   </si>
   <si>
-    <t>/b/o/t/</t>
+    <t>bot</t>
   </si>
   <si>
     <t>bought</t>
   </si>
   <si>
-    <t>/b/ɔ/t/</t>
+    <t>bɔt</t>
   </si>
   <si>
     <t>bob</t>
   </si>
   <si>
-    <t>/b/ɑ/b/</t>
+    <t>bɑb</t>
   </si>
   <si>
     <t>bite</t>
   </si>
   <si>
-    <t>/b/ɑɪ/t/</t>
+    <t>bɑɪt</t>
   </si>
   <si>
     <t>brown</t>
   </si>
   <si>
-    <t>/b/r/ɑʊ/n/</t>
+    <t>brɑʊn</t>
   </si>
   <si>
     <t>boy</t>
   </si>
   <si>
-    <t>/b/ɔɪ/</t>
+    <t>bɔɪ</t>
   </si>
   <si>
     <t>pot</t>
   </si>
   <si>
-    <t>/p/ɑ/t/</t>
+    <t>pɑt</t>
   </si>
   <si>
     <t>dog</t>
   </si>
   <si>
-    <t>/d/ɔ/g/</t>
+    <t>dɔg</t>
   </si>
   <si>
     <t>top</t>
   </si>
   <si>
-    <t>/t/ɑ/p/</t>
+    <t>tɑp</t>
   </si>
   <si>
     <t>kit</t>
   </si>
   <si>
-    <t>/k/ɪ/t/</t>
+    <t>kɪt</t>
   </si>
   <si>
     <t>got</t>
   </si>
   <si>
-    <t>/g/ɑ/t/</t>
+    <t>gɑt</t>
   </si>
   <si>
     <t>fog</t>
   </si>
   <si>
-    <t>/f/ɔ/g/</t>
+    <t>fɔg</t>
   </si>
   <si>
     <t>vat</t>
   </si>
   <si>
-    <t>/v/æ/t/</t>
+    <t>væt</t>
   </si>
   <si>
     <t>thick</t>
   </si>
   <si>
-    <t>/ɵ/ɪ/k/</t>
+    <t>ɵɪk</t>
   </si>
   <si>
     <t>that</t>
   </si>
   <si>
-    <t>/ð/æ/t/</t>
+    <t>ðæt</t>
   </si>
   <si>
     <t>sat</t>
   </si>
   <si>
-    <t>/s/æ/t/</t>
+    <t>sæt</t>
   </si>
   <si>
     <t>zoo</t>
   </si>
   <si>
-    <t>/z/u/</t>
+    <t>zu</t>
   </si>
   <si>
     <t>shut</t>
   </si>
   <si>
-    <t>/ʃ/ʌ/t/</t>
+    <t>ʃʌt</t>
   </si>
   <si>
     <t>measure</t>
   </si>
   <si>
-    <t>/m/ɛ/ʒ/ɚ/</t>
+    <t>mɛʒɚ</t>
   </si>
   <si>
     <t>help</t>
   </si>
   <si>
-    <t>/h/ɛ/l/p/</t>
+    <t>hɛlp</t>
   </si>
   <si>
     <t>church</t>
   </si>
   <si>
-    <t>/ʧ/ɚ/ʧ/</t>
+    <t>ʧɚʧ</t>
   </si>
   <si>
     <t>jump</t>
   </si>
   <si>
-    <t>/ʤ/ʌ/m/p/</t>
+    <t>ʤʌmp</t>
   </si>
   <si>
     <t>mom</t>
   </si>
   <si>
-    <t>/m/ɑ/m/</t>
+    <t>mɑm</t>
   </si>
   <si>
     <t>nod</t>
   </si>
   <si>
-    <t>/n/ɑ/d/</t>
+    <t>nɑd</t>
   </si>
   <si>
     <t>thing</t>
   </si>
   <si>
-    <t>/ɵ/ɪ/ŋ/</t>
+    <t>ɵɪŋ</t>
   </si>
   <si>
     <t>lot</t>
   </si>
   <si>
-    <t>/l/ɑ/t/</t>
+    <t>lɑt</t>
   </si>
   <si>
     <t>rat</t>
   </si>
   <si>
-    <t>/r/æ/t/</t>
+    <t>ræt</t>
   </si>
   <si>
     <t>won</t>
   </si>
   <si>
-    <t>/w/ʌ/n/</t>
+    <t>wʌn</t>
   </si>
   <si>
     <t>you</t>
   </si>
   <si>
-    <t>/j/u/</t>
+    <t>ju</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -510,22 +530,31 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF3C4858"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11.0"/>
       <color rgb="FF3C4858"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF3C4858"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
+      <sz val="12.0"/>
       <color rgb="FFFF0000"/>
-      <name val="Roboto"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -559,44 +588,51 @@
       </bottom>
     </border>
     <border>
+      <right/>
       <top style="thin">
         <color rgb="FFDDDDDD"/>
       </top>
+      <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,28 +667,28 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -811,14 +847,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +863,7 @@
       </c>
       <c r="P1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -835,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -843,7 +879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -851,7 +887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -859,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -867,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -875,7 +911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -883,7 +919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -891,7 +927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -899,7 +935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -907,7 +943,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -915,7 +951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -923,7 +959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -931,7 +967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -939,7 +975,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -947,7 +983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -955,7 +991,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -963,7 +999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -971,7 +1007,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -979,7 +1015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -987,7 +1023,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -995,7 +1031,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1003,7 +1039,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1011,7 +1047,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1019,7 +1055,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1027,7 +1063,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1035,7 +1071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -1043,7 +1079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -1051,7 +1087,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1059,7 +1095,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1067,7 +1103,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1075,7 +1111,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1083,7 +1119,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -1091,7 +1127,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -1099,7 +1135,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1107,7 +1143,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -1115,7 +1151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -1123,7 +1159,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -1131,7 +1167,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>78</v>
       </c>
@@ -1139,7 +1175,998 @@
         <v>79</v>
       </c>
     </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1147,414 +2174,1336 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="s">
+      <c r="B27" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="B31" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="7" t="s">
+      <c r="B32" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="5" t="s">
+      <c r="B33" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="7" t="s">
+      <c r="B35" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="10" t="s">
         <v>157</v>
       </c>
-    </row>
+      <c r="B38" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="9"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="C1"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
-    <hyperlink r:id="rId5" ref="C5"/>
-    <hyperlink r:id="rId6" ref="C6"/>
-    <hyperlink r:id="rId7" ref="C7"/>
-    <hyperlink r:id="rId8" ref="C8"/>
-    <hyperlink r:id="rId9" ref="C9"/>
-    <hyperlink r:id="rId10" ref="C10"/>
-    <hyperlink r:id="rId11" ref="C11"/>
-    <hyperlink r:id="rId12" ref="C12"/>
-    <hyperlink r:id="rId13" ref="C13"/>
-    <hyperlink r:id="rId14" ref="C14"/>
-    <hyperlink r:id="rId15" ref="C15"/>
-    <hyperlink r:id="rId16" ref="C16"/>
-    <hyperlink r:id="rId17" ref="C17"/>
-    <hyperlink r:id="rId18" ref="C18"/>
-    <hyperlink r:id="rId19" ref="C19"/>
-    <hyperlink r:id="rId20" ref="C20"/>
-    <hyperlink r:id="rId21" ref="C21"/>
-    <hyperlink r:id="rId22" ref="C22"/>
-    <hyperlink r:id="rId23" ref="C23"/>
-    <hyperlink r:id="rId24" ref="C24"/>
-    <hyperlink r:id="rId25" ref="C25"/>
-    <hyperlink r:id="rId26" ref="C26"/>
-    <hyperlink r:id="rId27" ref="C27"/>
-    <hyperlink r:id="rId28" ref="C28"/>
-    <hyperlink r:id="rId29" ref="C29"/>
-    <hyperlink r:id="rId30" ref="C30"/>
-    <hyperlink r:id="rId31" ref="C31"/>
-    <hyperlink r:id="rId32" ref="C32"/>
-    <hyperlink r:id="rId33" ref="C33"/>
-    <hyperlink r:id="rId34" ref="C34"/>
-    <hyperlink r:id="rId35" ref="C35"/>
-    <hyperlink r:id="rId36" ref="C36"/>
-    <hyperlink r:id="rId37" ref="C37"/>
-    <hyperlink r:id="rId38" ref="C38"/>
-    <hyperlink r:id="rId39" ref="C39"/>
-  </hyperlinks>
-  <drawing r:id="rId40"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>